<commit_message>
Revert "Revert "Merge branch 'master' into USA_Rework""
This reverts commit 0e8fbf8d22aa74586c255929da2cb221c9319874.
</commit_message>
<xml_diff>
--- a/WIP/Aces Sheet.xlsx
+++ b/WIP/Aces Sheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{91DBE264-5F92-49C8-8572-D524F5CCFB3A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED209CA8-681E-4B21-8BA3-342D7BBDF615}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
-  <si>
-    <t>https://en.wikipedia.org/wiki/Erich_Hartmann</t>
-  </si>
-  <si>
-    <t>42-43</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="84">
   <si>
     <t>Me109G</t>
   </si>
@@ -185,6 +179,99 @@
   </si>
   <si>
     <t>40-46</t>
+  </si>
+  <si>
+    <t>Gerhard Barkhorn</t>
+  </si>
+  <si>
+    <t>Günther Rall</t>
+  </si>
+  <si>
+    <t>Otto Kittel</t>
+  </si>
+  <si>
+    <t>Walter Nowotny</t>
+  </si>
+  <si>
+    <t>Wilhelm Batz</t>
+  </si>
+  <si>
+    <t>Erich Rudorffer</t>
+  </si>
+  <si>
+    <t>41-45</t>
+  </si>
+  <si>
+    <t>42-45</t>
+  </si>
+  <si>
+    <t>FW190</t>
+  </si>
+  <si>
+    <t>41-45KIA</t>
+  </si>
+  <si>
+    <t>41-44KIA</t>
+  </si>
+  <si>
+    <t>43-45</t>
+  </si>
+  <si>
+    <t>Richard I. Bong</t>
+  </si>
+  <si>
+    <t>Thomas B. McGuire</t>
+  </si>
+  <si>
+    <t>David McCampbell</t>
+  </si>
+  <si>
+    <t>Francis "Gabby" Gabreski</t>
+  </si>
+  <si>
+    <t>Gregory "Pappy" Boyington</t>
+  </si>
+  <si>
+    <t>Robert S. Johnson</t>
+  </si>
+  <si>
+    <t>Charles H. MacDonald</t>
+  </si>
+  <si>
+    <t>George E. Preddy, Jr.</t>
+  </si>
+  <si>
+    <t>Joseph J. Foss</t>
+  </si>
+  <si>
+    <t>Robert M. Hanson</t>
+  </si>
+  <si>
+    <t>Neel E. Kearby</t>
+  </si>
+  <si>
+    <t>Ivan Kozhedub</t>
+  </si>
+  <si>
+    <t>Lev Shestakov</t>
+  </si>
+  <si>
+    <t>Aleksandr Ivanovich Pokryshkin</t>
+  </si>
+  <si>
+    <t>Grigoriy Andreevich Rechkalov</t>
+  </si>
+  <si>
+    <t>Nikolay Dmitrievich Gulayev</t>
+  </si>
+  <si>
+    <t>Kirill A. Yevstigneyev</t>
+  </si>
+  <si>
+    <t>Dmitri Hlinka</t>
+  </si>
+  <si>
+    <t>Ivan Babak</t>
   </si>
 </sst>
 </file>
@@ -325,7 +412,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -342,15 +429,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1"/>
@@ -372,6 +450,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
@@ -657,928 +748,990 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.54296875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8"/>
-      <c r="L2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="19"/>
+      <c r="L2" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="19"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="N3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="O3" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="P3" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="L5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="L6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="L8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="L9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>59</v>
+      </c>
       <c r="L10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="L11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="13" t="s">
+        <v>66</v>
+      </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="L12" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="13" t="s">
+        <v>67</v>
+      </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="L13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="13" t="s">
+        <v>68</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="L14" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="13" t="s">
+        <v>69</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="L15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="13" t="s">
+        <v>70</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="L16" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+      <c r="D17" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="L17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="L18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
+      <c r="D19" s="13" t="s">
+        <v>73</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
-      <c r="L19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="L20" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B21" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
       <c r="L21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="13" t="s">
+        <v>76</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="L22" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="13" t="s">
+        <v>77</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="L23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="D24" s="13" t="s">
+        <v>78</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="L24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
+      <c r="D25" s="13" t="s">
+        <v>79</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="L25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="D26" s="13" t="s">
+        <v>80</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="L26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+      <c r="D27" s="13" t="s">
+        <v>81</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="L27" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-      <c r="P27" s="14"/>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="D28" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="L28" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B29" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="11"/>
+      <c r="D29" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
       <c r="L29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="L30" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="L30" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
       <c r="L31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
       <c r="L32" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="L33" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="L34" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="12"/>
-    </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="L34" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="L35" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
       <c r="L36" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
       <c r="L37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
       <c r="L38" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="L39" s="13" t="s">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="L39" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B40" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="L40" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N40" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P40" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="L41" t="s">
+        <v>20</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N41" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="L42" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N42" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P42" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="L43" t="s">
+        <v>20</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N43" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P43" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="L44" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M44" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="N44" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="O44" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="P44" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B45" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="L45" t="s">
         <v>21</v>
       </c>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="L40" s="5" t="s">
+      <c r="M45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N45" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="L46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M46" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N46" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O46" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="P46" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="L47" t="s">
         <v>22</v>
       </c>
-      <c r="M40" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N40" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="O40" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P40" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>14</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="L41" t="s">
+      <c r="M47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N47" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B48" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="L48" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="M41" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="N41" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="O41" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="P41" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="L42" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="N42" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="O42" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P42" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B43" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="L43" t="s">
-        <v>22</v>
-      </c>
-      <c r="M43" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N43" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="O43" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P43" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="L44" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M44" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="N44" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="O44" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="P44" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="L45" t="s">
+      <c r="M48" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N48" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O48" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="P48" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="L49" t="s">
         <v>23</v>
       </c>
-      <c r="M45" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N45" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="O45" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P45" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B46" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="L46" s="15" t="s">
+      <c r="M49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="12:16" x14ac:dyDescent="0.35">
+      <c r="L50" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="M46" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N46" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="O46" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="P46" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>15</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="L47" t="s">
-        <v>24</v>
-      </c>
-      <c r="M47" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N47" s="18" t="s">
+      <c r="M50" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N50" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O50" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="P50" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="O47" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="L48" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="M48" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N48" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="O48" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="P48" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="L49" t="s">
-        <v>25</v>
-      </c>
-      <c r="M49" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N49" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="O49" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P49" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="L50" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="M50" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N50" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="O50" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="P50" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B51" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
+    </row>
+    <row r="51" spans="12:16" x14ac:dyDescent="0.35">
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
@@ -1601,8 +1754,34 @@
     <hyperlink ref="N44" r:id="rId9" tooltip="Mark Henry Brown" display="https://en.wikipedia.org/wiki/Mark_Henry_Brown" xr:uid="{6E5DE38C-EA94-42A4-BBA8-813D30D69487}"/>
     <hyperlink ref="N45" r:id="rId10" tooltip="Marmaduke Pattle" display="https://en.wikipedia.org/wiki/Marmaduke_Pattle" xr:uid="{012ECC22-2108-421E-B35F-F56B9B47542E}"/>
     <hyperlink ref="N46" r:id="rId11" tooltip="Adolph Malan" display="https://en.wikipedia.org/wiki/Adolph_Malan" xr:uid="{F89CF312-8468-4D45-A909-FFC4414C8EF4}"/>
+    <hyperlink ref="D4" r:id="rId12" xr:uid="{0FC95589-0B49-4B54-A1AE-57F3C45A9559}"/>
+    <hyperlink ref="D5" r:id="rId13" display="https://en.wikipedia.org/wiki/Gerhard_Barkhorn" xr:uid="{01F8CCB4-216F-4EB7-9077-6E5A1B2CD921}"/>
+    <hyperlink ref="D6" r:id="rId14" display="https://en.wikipedia.org/wiki/G%C3%BCnther_Rall" xr:uid="{84E72A0F-D982-4562-B242-31F811C7A77E}"/>
+    <hyperlink ref="D7" r:id="rId15" display="https://en.wikipedia.org/wiki/Otto_Kittel" xr:uid="{F0780AC8-7E29-4322-8D79-957742D498C6}"/>
+    <hyperlink ref="D8" r:id="rId16" display="https://en.wikipedia.org/wiki/Walter_Nowotny" xr:uid="{0C4EECB4-713F-4BA9-9839-4CDFBCAD1CEC}"/>
+    <hyperlink ref="D9" r:id="rId17" display="https://en.wikipedia.org/wiki/Wilhelm_Batz" xr:uid="{AC1386B3-93ED-4868-905B-ABC69B42602A}"/>
+    <hyperlink ref="D10" r:id="rId18" display="https://en.wikipedia.org/wiki/Erich_Rudorffer" xr:uid="{F5AE1303-3237-45B7-9AC0-D42BA3A34299}"/>
+    <hyperlink ref="D11" r:id="rId19" display="https://en.wikipedia.org/wiki/Richard_Bong" xr:uid="{DD059D6E-45A3-4281-A9AB-3226A58D1690}"/>
+    <hyperlink ref="D12" r:id="rId20" display="https://en.wikipedia.org/wiki/Thomas_McGuire" xr:uid="{3CC29DD6-DBA7-4C63-A186-97639E5D5A22}"/>
+    <hyperlink ref="D13" r:id="rId21" display="https://en.wikipedia.org/wiki/David_McCampbell" xr:uid="{8D9EC7BE-5CBF-4F78-A3AB-715084753399}"/>
+    <hyperlink ref="D14" r:id="rId22" display="https://en.wikipedia.org/wiki/Francis_S._Gabreski" xr:uid="{3FC6107B-4180-4B5E-9364-43549DA5CC94}"/>
+    <hyperlink ref="D15" r:id="rId23" display="https://en.wikipedia.org/wiki/Pappy_Boyington" xr:uid="{D0F09119-DA02-4FAF-A876-96E8E67F40B9}"/>
+    <hyperlink ref="D16" r:id="rId24" display="https://en.wikipedia.org/wiki/Robert_S._Johnson" xr:uid="{1484969E-5F90-4C73-8BD9-83EA10F52588}"/>
+    <hyperlink ref="D17" r:id="rId25" display="https://en.wikipedia.org/wiki/Charles_H._MacDonald" xr:uid="{9AEF9967-5391-4E88-A4A4-93AD7CC441D5}"/>
+    <hyperlink ref="D18" r:id="rId26" display="https://en.wikipedia.org/wiki/George_Preddy" xr:uid="{AA03BEB2-8934-40D8-AF5C-778330026D18}"/>
+    <hyperlink ref="D19" r:id="rId27" display="https://en.wikipedia.org/wiki/Joseph_J._Foss" xr:uid="{2EDA10BB-1EDF-44F1-BC3E-4AFBE68462CC}"/>
+    <hyperlink ref="D20" r:id="rId28" display="https://en.wikipedia.org/wiki/Robert_M._Hanson" xr:uid="{0B487446-7872-4E04-93C1-AA5A3D92D51F}"/>
+    <hyperlink ref="D21" r:id="rId29" display="https://en.wikipedia.org/wiki/Neel_E._Kearby" xr:uid="{345A9172-55D8-4773-A82F-2088E0D08C0E}"/>
+    <hyperlink ref="D22" r:id="rId30" display="https://en.wikipedia.org/wiki/Ivan_Kozhedub" xr:uid="{931C0B6E-8872-44BB-B2DD-7ADC48EE7DEE}"/>
+    <hyperlink ref="D23" r:id="rId31" display="https://en.wikipedia.org/wiki/Lev_Shestakov" xr:uid="{07D10C2A-D9E9-4B41-9AD0-DBD411B65129}"/>
+    <hyperlink ref="D24" r:id="rId32" display="https://en.wikipedia.org/wiki/Aleksandr_Ivanovich_Pokryshkin" xr:uid="{6C4EB317-1834-46F3-8A99-07571EE8FA89}"/>
+    <hyperlink ref="D25" r:id="rId33" display="https://en.wikipedia.org/wiki/Grigoriy_Andreevich_Rechkalov" xr:uid="{167C201E-5FE2-40E7-9351-2B12C301BD02}"/>
+    <hyperlink ref="D26" r:id="rId34" display="https://en.wikipedia.org/wiki/Nikolay_Dmitrievich_Gulayev" xr:uid="{0140EAD4-33E8-43C8-A2D5-140735857F80}"/>
+    <hyperlink ref="D27" r:id="rId35" display="https://en.wikipedia.org/wiki/Kirill_A._Yevstigneyev" xr:uid="{206E0B6A-FC5C-43B6-997C-13D187DB33BC}"/>
+    <hyperlink ref="D28" r:id="rId36" display="https://en.wikipedia.org/wiki/Dmitri_Glinka" xr:uid="{BAB9A44F-1922-4773-8CBE-D51EE73D02A7}"/>
+    <hyperlink ref="D29" r:id="rId37" display="https://en.wikipedia.org/wiki/Ivan_Babak" xr:uid="{FB7733A3-A3D5-496E-8710-6C84A8CE0180}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes to AAA & Art Locs GER
</commit_message>
<xml_diff>
--- a/WIP/Aces Sheet.xlsx
+++ b/WIP/Aces Sheet.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED209CA8-681E-4B21-8BA3-342D7BBDF615}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9507CCE5-A64E-4D02-A1CB-0864BAF239C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="90">
   <si>
     <t>Me109G</t>
   </si>
@@ -272,6 +272,24 @@
   </si>
   <si>
     <t>Ivan Babak</t>
+  </si>
+  <si>
+    <t>William Vale</t>
+  </si>
+  <si>
+    <t>James Edgar "Johnnie" Johnson</t>
+  </si>
+  <si>
+    <t>Robert Roland Stanford Tuck</t>
+  </si>
+  <si>
+    <t>Bob Braham</t>
+  </si>
+  <si>
+    <t>"Ginger" Lacey</t>
+  </si>
+  <si>
+    <t>Neville Duke</t>
   </si>
 </sst>
 </file>
@@ -450,6 +468,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,10 +481,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="2" builtinId="39"/>
@@ -748,35 +766,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
-      <c r="L2" s="17" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="L2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="19"/>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="21"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
@@ -808,14 +826,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="17" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -832,7 +850,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -856,7 +874,7 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
@@ -880,7 +898,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -904,7 +922,7 @@
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
@@ -928,7 +946,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -952,7 +970,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>3</v>
       </c>
@@ -976,7 +994,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -994,7 +1012,7 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1012,7 +1030,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -1030,7 +1048,7 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1066,7 @@
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -1066,7 +1084,7 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
@@ -1084,7 +1102,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1120,7 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
@@ -1120,7 +1138,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>10</v>
       </c>
@@ -1138,7 +1156,7 @@
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>10</v>
       </c>
@@ -1156,7 +1174,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
         <v>10</v>
       </c>
@@ -1174,7 +1192,7 @@
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
         <v>11</v>
       </c>
@@ -1192,7 +1210,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>11</v>
       </c>
@@ -1210,7 +1228,7 @@
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1228,7 +1246,7 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>11</v>
       </c>
@@ -1246,7 +1264,7 @@
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1282,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>11</v>
       </c>
@@ -1282,7 +1300,7 @@
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>11</v>
       </c>
@@ -1300,12 +1318,12 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="11"/>
-      <c r="D29" s="21" t="s">
+      <c r="D29" s="18" t="s">
         <v>83</v>
       </c>
       <c r="E29" s="11"/>
@@ -1318,12 +1336,14 @@
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
+      <c r="D30" s="13" t="s">
+        <v>84</v>
+      </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="L30" s="8" t="s">
@@ -1334,12 +1354,14 @@
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="D31" s="13" t="s">
+        <v>85</v>
+      </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="L31" t="s">
@@ -1350,12 +1372,14 @@
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="13" t="s">
+        <v>86</v>
+      </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="L32" s="2" t="s">
@@ -1366,12 +1390,14 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
+      <c r="D33" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="L33" t="s">
@@ -1382,12 +1408,14 @@
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
+      <c r="D34" s="13" t="s">
+        <v>88</v>
+      </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="L34" s="8" t="s">
@@ -1398,12 +1426,14 @@
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="D35" s="13" t="s">
+        <v>89</v>
+      </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="L35" t="s">
@@ -1414,7 +1444,7 @@
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>12</v>
       </c>
@@ -1430,7 +1460,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>12</v>
       </c>
@@ -1446,7 +1476,7 @@
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>12</v>
       </c>
@@ -1462,7 +1492,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>12</v>
       </c>
@@ -1478,7 +1508,7 @@
       <c r="O39" s="11"/>
       <c r="P39" s="11"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="10" t="s">
         <v>12</v>
       </c>
@@ -1502,7 +1532,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
         <v>13</v>
       </c>
@@ -1526,7 +1556,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>13</v>
       </c>
@@ -1550,7 +1580,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>13</v>
       </c>
@@ -1574,7 +1604,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>13</v>
       </c>
@@ -1598,7 +1628,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>13</v>
       </c>
@@ -1622,7 +1652,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>13</v>
       </c>
@@ -1646,7 +1676,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>13</v>
       </c>
@@ -1673,7 +1703,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
         <v>13</v>
       </c>
@@ -1697,7 +1727,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="49" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L49" t="s">
         <v>23</v>
       </c>
@@ -1714,7 +1744,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="50" spans="12:16" x14ac:dyDescent="0.25">
       <c r="L50" s="12" t="s">
         <v>23</v>
       </c>
@@ -1731,7 +1761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="12:16" x14ac:dyDescent="0.35">
+    <row r="51" spans="12:16" x14ac:dyDescent="0.25">
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
@@ -1780,8 +1810,14 @@
     <hyperlink ref="D27" r:id="rId35" display="https://en.wikipedia.org/wiki/Kirill_A._Yevstigneyev" xr:uid="{206E0B6A-FC5C-43B6-997C-13D187DB33BC}"/>
     <hyperlink ref="D28" r:id="rId36" display="https://en.wikipedia.org/wiki/Dmitri_Glinka" xr:uid="{BAB9A44F-1922-4773-8CBE-D51EE73D02A7}"/>
     <hyperlink ref="D29" r:id="rId37" display="https://en.wikipedia.org/wiki/Ivan_Babak" xr:uid="{FB7733A3-A3D5-496E-8710-6C84A8CE0180}"/>
+    <hyperlink ref="D30" r:id="rId38" display="https://en.wikipedia.org/wiki/William_Vale" xr:uid="{BA4FD674-9832-4CC7-93AF-FFACFA3CD225}"/>
+    <hyperlink ref="D31" r:id="rId39" display="https://en.wikipedia.org/wiki/Johnnie_Johnson_(pilot)" xr:uid="{1919F597-5EEF-42D5-AA0B-C5D62586AE22}"/>
+    <hyperlink ref="D32" r:id="rId40" tooltip="Robert Stanford Tuck" display="https://en.wikipedia.org/wiki/Robert_Stanford_Tuck" xr:uid="{867B4C4A-D7C6-417B-A8EC-55AC7847A3B2}"/>
+    <hyperlink ref="D33" r:id="rId41" tooltip="Bob Braham" display="https://en.wikipedia.org/wiki/Bob_Braham" xr:uid="{2ADDAB17-E12C-4D31-BE0A-300E50EE5FB6}"/>
+    <hyperlink ref="D34" r:id="rId42" tooltip="James Harry Lacey" display="https://en.wikipedia.org/wiki/James_Harry_Lacey" xr:uid="{AC9496C8-BD07-4534-AA75-D5EED4FFD53A}"/>
+    <hyperlink ref="D35" r:id="rId43" tooltip="Neville Duke" display="https://en.wikipedia.org/wiki/Neville_Duke" xr:uid="{48619FDB-628C-4DD1-98D8-BD39D32630FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
UK Aces, ITA & JAPs soon
</commit_message>
<xml_diff>
--- a/WIP/Aces Sheet.xlsx
+++ b/WIP/Aces Sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9507CCE5-A64E-4D02-A1CB-0864BAF239C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AEF2C7-EABE-4F57-B685-1639020D8B39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="101">
   <si>
     <t>Me109G</t>
   </si>
@@ -290,6 +290,39 @@
   </si>
   <si>
     <t>Neville Duke</t>
+  </si>
+  <si>
+    <t>Teresio Vittorio Martinoli</t>
+  </si>
+  <si>
+    <t>Leonardo Ferrulli</t>
+  </si>
+  <si>
+    <t>Franco Lucchini</t>
+  </si>
+  <si>
+    <t>Franco Bordoni</t>
+  </si>
+  <si>
+    <t>Luigi Gorrini</t>
+  </si>
+  <si>
+    <t>Tetsuzo Iwamoto</t>
+  </si>
+  <si>
+    <t>Shigeo Fukumoto</t>
+  </si>
+  <si>
+    <t>Shoichi Sugita</t>
+  </si>
+  <si>
+    <t>Hiromichi Shinohara</t>
+  </si>
+  <si>
+    <t>Takeo Okumura</t>
+  </si>
+  <si>
+    <t>Satoru Anabuki</t>
   </si>
 </sst>
 </file>
@@ -766,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,7 +879,9 @@
         <v>14</v>
       </c>
       <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="N4" s="13" t="s">
+        <v>95</v>
+      </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
@@ -870,7 +905,9 @@
         <v>14</v>
       </c>
       <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
+      <c r="N5" s="13" t="s">
+        <v>96</v>
+      </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
@@ -894,7 +931,9 @@
         <v>14</v>
       </c>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+      <c r="N6" s="13" t="s">
+        <v>97</v>
+      </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
@@ -918,7 +957,9 @@
         <v>14</v>
       </c>
       <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
+      <c r="N7" s="13" t="s">
+        <v>98</v>
+      </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
     </row>
@@ -942,7 +983,9 @@
         <v>14</v>
       </c>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+      <c r="N8" s="13" t="s">
+        <v>99</v>
+      </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
@@ -966,7 +1009,9 @@
         <v>14</v>
       </c>
       <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="N9" s="13" t="s">
+        <v>100</v>
+      </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
@@ -1537,7 +1582,9 @@
         <v>13</v>
       </c>
       <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="D41" s="13" t="s">
+        <v>90</v>
+      </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="L41" t="s">
@@ -1561,7 +1608,9 @@
         <v>13</v>
       </c>
       <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
+      <c r="D42" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="L42" s="2" t="s">
@@ -1585,7 +1634,9 @@
         <v>13</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="D43" s="13" t="s">
+        <v>92</v>
+      </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="L43" t="s">
@@ -1609,7 +1660,9 @@
         <v>13</v>
       </c>
       <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="D44" s="13" t="s">
+        <v>93</v>
+      </c>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="L44" s="8" t="s">
@@ -1633,7 +1686,9 @@
         <v>13</v>
       </c>
       <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="D45" s="13" t="s">
+        <v>94</v>
+      </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="L45" t="s">
@@ -1816,8 +1871,19 @@
     <hyperlink ref="D33" r:id="rId41" tooltip="Bob Braham" display="https://en.wikipedia.org/wiki/Bob_Braham" xr:uid="{2ADDAB17-E12C-4D31-BE0A-300E50EE5FB6}"/>
     <hyperlink ref="D34" r:id="rId42" tooltip="James Harry Lacey" display="https://en.wikipedia.org/wiki/James_Harry_Lacey" xr:uid="{AC9496C8-BD07-4534-AA75-D5EED4FFD53A}"/>
     <hyperlink ref="D35" r:id="rId43" tooltip="Neville Duke" display="https://en.wikipedia.org/wiki/Neville_Duke" xr:uid="{48619FDB-628C-4DD1-98D8-BD39D32630FB}"/>
+    <hyperlink ref="D41" r:id="rId44" display="https://en.wikipedia.org/wiki/Teresio_Vittorio_Martinoli" xr:uid="{F7823089-0CC1-4CF4-9665-DFEB1E8DF082}"/>
+    <hyperlink ref="D42" r:id="rId45" display="https://en.wikipedia.org/wiki/Leonardo_Ferrulli" xr:uid="{E8E25CDB-5153-4D21-A550-B72D59CCB546}"/>
+    <hyperlink ref="D43" r:id="rId46" display="https://en.wikipedia.org/wiki/Franco_Lucchini" xr:uid="{532A3372-D4E9-43A8-AA87-F119BE85B56A}"/>
+    <hyperlink ref="D44" r:id="rId47" display="https://en.wikipedia.org/wiki/Franco_Bordoni" xr:uid="{5291F778-1106-433D-ABC9-DE2571259811}"/>
+    <hyperlink ref="D45" r:id="rId48" display="https://en.wikipedia.org/wiki/Luigi_Gorrini" xr:uid="{B4B72933-B5CE-47DD-BD62-3BA774FFFD86}"/>
+    <hyperlink ref="N4" r:id="rId49" display="https://en.wikipedia.org/wiki/Tetsuzo_Iwamoto" xr:uid="{C6B588E5-D586-4F15-9470-A059BD8D6876}"/>
+    <hyperlink ref="N5" r:id="rId50" tooltip="Shigeo Fukumoto (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Shigeo_Fukumoto&amp;action=edit&amp;redlink=1" xr:uid="{8C3F4A41-9AF7-4466-82F0-6580ED90D947}"/>
+    <hyperlink ref="N6" r:id="rId51" tooltip="Shoichi Sugita (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Shoichi_Sugita&amp;action=edit&amp;redlink=1" xr:uid="{ED5749F6-35BD-45AD-8C6C-07DE73E87937}"/>
+    <hyperlink ref="N7" r:id="rId52" display="https://en.wikipedia.org/wiki/Hiromichi_Shinohara" xr:uid="{BA13E48C-AD64-47CA-99CD-380E073018D5}"/>
+    <hyperlink ref="N8" r:id="rId53" display="https://en.wikipedia.org/wiki/Takeo_Okumura" xr:uid="{55A40192-040D-4E48-BDBC-25D7DD79A577}"/>
+    <hyperlink ref="N9" r:id="rId54" display="https://en.wikipedia.org/wiki/Satoru_Anabuki" xr:uid="{B7580199-D7FA-425D-977C-A48D7A24A6D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId44"/>
+  <pageSetup orientation="portrait" r:id="rId55"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SS Totenkopf fix & JAP SNLF
</commit_message>
<xml_diff>
--- a/WIP/Aces Sheet.xlsx
+++ b/WIP/Aces Sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AEF2C7-EABE-4F57-B685-1639020D8B39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D56F06-28DC-4853-B004-CC903272D6D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -310,12 +310,6 @@
     <t>Tetsuzo Iwamoto</t>
   </si>
   <si>
-    <t>Shigeo Fukumoto</t>
-  </si>
-  <si>
-    <t>Shoichi Sugita</t>
-  </si>
-  <si>
     <t>Hiromichi Shinohara</t>
   </si>
   <si>
@@ -323,6 +317,12 @@
   </si>
   <si>
     <t>Satoru Anabuki</t>
+  </si>
+  <si>
+    <t>Hiroyoshi Nishizawa</t>
+  </si>
+  <si>
+    <t>Toshio Ota</t>
   </si>
 </sst>
 </file>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,7 +906,7 @@
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="13" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -932,7 +932,7 @@
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="13" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -958,7 +958,7 @@
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
@@ -984,7 +984,7 @@
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -1877,11 +1877,11 @@
     <hyperlink ref="D44" r:id="rId47" display="https://en.wikipedia.org/wiki/Franco_Bordoni" xr:uid="{5291F778-1106-433D-ABC9-DE2571259811}"/>
     <hyperlink ref="D45" r:id="rId48" display="https://en.wikipedia.org/wiki/Luigi_Gorrini" xr:uid="{B4B72933-B5CE-47DD-BD62-3BA774FFFD86}"/>
     <hyperlink ref="N4" r:id="rId49" display="https://en.wikipedia.org/wiki/Tetsuzo_Iwamoto" xr:uid="{C6B588E5-D586-4F15-9470-A059BD8D6876}"/>
-    <hyperlink ref="N5" r:id="rId50" tooltip="Shigeo Fukumoto (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Shigeo_Fukumoto&amp;action=edit&amp;redlink=1" xr:uid="{8C3F4A41-9AF7-4466-82F0-6580ED90D947}"/>
-    <hyperlink ref="N6" r:id="rId51" tooltip="Shoichi Sugita (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Shoichi_Sugita&amp;action=edit&amp;redlink=1" xr:uid="{ED5749F6-35BD-45AD-8C6C-07DE73E87937}"/>
-    <hyperlink ref="N7" r:id="rId52" display="https://en.wikipedia.org/wiki/Hiromichi_Shinohara" xr:uid="{BA13E48C-AD64-47CA-99CD-380E073018D5}"/>
-    <hyperlink ref="N8" r:id="rId53" display="https://en.wikipedia.org/wiki/Takeo_Okumura" xr:uid="{55A40192-040D-4E48-BDBC-25D7DD79A577}"/>
-    <hyperlink ref="N9" r:id="rId54" display="https://en.wikipedia.org/wiki/Satoru_Anabuki" xr:uid="{B7580199-D7FA-425D-977C-A48D7A24A6D1}"/>
+    <hyperlink ref="N7" r:id="rId50" display="https://en.wikipedia.org/wiki/Hiromichi_Shinohara" xr:uid="{BA13E48C-AD64-47CA-99CD-380E073018D5}"/>
+    <hyperlink ref="N8" r:id="rId51" display="https://en.wikipedia.org/wiki/Takeo_Okumura" xr:uid="{55A40192-040D-4E48-BDBC-25D7DD79A577}"/>
+    <hyperlink ref="N9" r:id="rId52" display="https://en.wikipedia.org/wiki/Satoru_Anabuki" xr:uid="{B7580199-D7FA-425D-977C-A48D7A24A6D1}"/>
+    <hyperlink ref="N5" r:id="rId53" display="https://en.wikipedia.org/wiki/Hiroyoshi_Nishizawa" xr:uid="{C7BA1949-461F-4CFF-8BBE-23B613E57D60}"/>
+    <hyperlink ref="N6" r:id="rId54" display="https://en.wikipedia.org/wiki/Toshio_Ota" xr:uid="{960E047F-061A-4DE6-B4E7-C7A6EC69C654}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId55"/>

</xml_diff>